<commit_message>
[Timesheet Calculator v2] fixed the bug that computes the credited minutes and excess minutes during creation of employee spreadsheet. fixed testdata.
</commit_message>
<xml_diff>
--- a/python_source/Timesheet Calculator v2/Timesheet Calculator v2/test/business_logic/testdata/ss_generator_testdata_001.xlsx
+++ b/python_source/Timesheet Calculator v2/Timesheet Calculator v2/test/business_logic/testdata/ss_generator_testdata_001.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="48">
   <si>
     <t xml:space="preserve">PTCC TIMESHEET FOR WEEK (07-Jun-2021 to 21-Jun-2021)</t>
   </si>
@@ -168,6 +168,12 @@
   </si>
   <si>
     <t xml:space="preserve">20-Jun-2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WEEK COVERED: 21-Jun-2021 to 21-Jun-2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21-Jun-2021</t>
   </si>
 </sst>
 </file>
@@ -179,7 +185,7 @@
     <numFmt numFmtId="165" formatCode="#,##0.00"/>
     <numFmt numFmtId="166" formatCode="dd/mmm/yyyy"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -208,6 +214,12 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -251,7 +263,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -277,6 +289,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -299,11 +319,11 @@
   </sheetPr>
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="50.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="80.9"/>
@@ -414,13 +434,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D33" activeCellId="0" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="44.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.62"/>
@@ -737,10 +757,10 @@
         <v>120</v>
       </c>
       <c r="E22" s="6" t="n">
-        <v>480</v>
+        <v>0</v>
       </c>
       <c r="F22" s="0" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -757,6 +777,49 @@
         <v>0</v>
       </c>
       <c r="F23" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F27" s="8" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Timesheet Calculator v2] updated testdata to current date to pass the test.
</commit_message>
<xml_diff>
--- a/python_source/Timesheet Calculator v2/Timesheet Calculator v2/test/business_logic/testdata/ss_generator_testdata_001.xlsx
+++ b/python_source/Timesheet Calculator v2/Timesheet Calculator v2/test/business_logic/testdata/ss_generator_testdata_001.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,7 +26,7 @@
     <t xml:space="preserve">PTCC TIMESHEET FOR WEEK (07-Jun-2021 to 21-Jun-2021)</t>
   </si>
   <si>
-    <t xml:space="preserve">16-June-2021</t>
+    <t xml:space="preserve">08-July-2021</t>
   </si>
   <si>
     <t xml:space="preserve">NAME</t>
@@ -319,11 +319,11 @@
   </sheetPr>
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="50.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="80.9"/>
@@ -436,11 +436,11 @@
   </sheetPr>
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D33" activeCellId="0" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="44.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.62"/>

</xml_diff>